<commit_message>
update CarList to use RTK Query
</commit_message>
<xml_diff>
--- a/ExcelFiles/InvoiceReport.xlsx
+++ b/ExcelFiles/InvoiceReport.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Firma testowa</t>
+  </si>
+  <si>
+    <t>AK AK</t>
   </si>
   <si>
     <t>https://www.e-iceblue.com/Buy/Spire.XLS.html</t>
@@ -554,7 +557,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -846,6 +849,166 @@
       </c>
       <c r="F14" s="1">
         <v>45322</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="12.75">
+      <c r="A15">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>420</v>
+      </c>
+      <c r="D15">
+        <v>420</v>
+      </c>
+      <c r="E15" s="1">
+        <v>45331</v>
+      </c>
+      <c r="F15" s="1">
+        <v>45331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="12.75">
+      <c r="A16">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>750</v>
+      </c>
+      <c r="D16">
+        <v>750</v>
+      </c>
+      <c r="E16" s="1">
+        <v>45333.488132211896</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45333.488132212464</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="12.75">
+      <c r="A17">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>500</v>
+      </c>
+      <c r="D17">
+        <v>500</v>
+      </c>
+      <c r="E17" s="1">
+        <v>45333.50467125974</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45333.50467125977</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="12.75">
+      <c r="A18">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>250</v>
+      </c>
+      <c r="D18">
+        <v>250</v>
+      </c>
+      <c r="E18" s="1">
+        <v>45333.52913617004</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45333.529136170066</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="12.75">
+      <c r="A19">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>450</v>
+      </c>
+      <c r="D19">
+        <v>450</v>
+      </c>
+      <c r="E19" s="1">
+        <v>45337.634505044945</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45337.634505045404</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="12.75">
+      <c r="A20">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>720</v>
+      </c>
+      <c r="D20">
+        <v>720</v>
+      </c>
+      <c r="E20" s="1">
+        <v>45337.75045813944</v>
+      </c>
+      <c r="F20" s="1">
+        <v>45337.7504581405</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="12.75">
+      <c r="A21">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>960</v>
+      </c>
+      <c r="D21">
+        <v>960</v>
+      </c>
+      <c r="E21" s="1">
+        <v>45337.754077653444</v>
+      </c>
+      <c r="F21" s="1">
+        <v>45337.75407765347</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="12.75">
+      <c r="A22">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>420</v>
+      </c>
+      <c r="D22">
+        <v>420</v>
+      </c>
+      <c r="E22" s="1">
+        <v>45413.52797942728</v>
+      </c>
+      <c r="F22" s="1">
+        <v>45413.527979429186</v>
       </c>
     </row>
   </sheetData>
@@ -893,42 +1056,42 @@
   <sheetData>
     <row r="1" ht="12.75">
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" ht="12.75">
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" ht="12.75">
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" ht="12.75">
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" ht="12.75">
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" ht="12.75">
       <c r="B8" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" ht="12.75">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" ht="12.75">
       <c r="B11" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>